<commit_message>
feat: Codigo para correr todos los otros
</commit_message>
<xml_diff>
--- a/data/segmentacion.xlsx
+++ b/data/segmentacion.xlsx
@@ -1,31 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebatoec/tests/xlwings/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebatoec/projects/plantilla_seguimiento/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{321C0BFF-E7DD-1647-9AA3-BF1A6F52FFF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6895AEDE-472D-E641-94ED-39D8F004E723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17340" activeTab="5" xr2:uid="{50E09FA1-93C2-8744-880E-4EAF34B822D2}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17340" activeTab="4" xr2:uid="{50E09FA1-93C2-8744-880E-4EAF34B822D2}"/>
   </bookViews>
   <sheets>
-    <sheet name="add_Polizas" sheetId="8" r:id="rId1"/>
-    <sheet name="add_Canales" sheetId="9" r:id="rId2"/>
-    <sheet name="add_Amparos" sheetId="1" r:id="rId3"/>
-    <sheet name="add_Serfi" sheetId="11" r:id="rId4"/>
-    <sheet name="add_Atipicos" sheetId="13" r:id="rId5"/>
+    <sheet name="add_spe_Polizas" sheetId="8" r:id="rId1"/>
+    <sheet name="add_spe_Canales" sheetId="9" r:id="rId2"/>
+    <sheet name="add_spe_Amparos" sheetId="1" r:id="rId3"/>
+    <sheet name="add_spe_Serfi" sheetId="11" r:id="rId4"/>
+    <sheet name="add_s_Atipicos" sheetId="13" r:id="rId5"/>
     <sheet name="Fechas" sheetId="12" r:id="rId6"/>
     <sheet name="Cuadre_Contable_Siniestros" sheetId="14" r:id="rId7"/>
     <sheet name="Cuadre_Contable_Primas" sheetId="15" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">add_Amparos!$C$1:$G$112</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">add_Canales!$C$1:$F$2519</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">add_Polizas!$B$1:$D$18</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">add_spe_Amparos!$C$1:$G$112</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">add_spe_Canales!$C$1:$F$2519</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">add_spe_Polizas!$B$1:$D$18</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -3673,7 +3673,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -27712,8 +27712,8 @@
   <sheetPr codeName="Hoja6"/>
   <dimension ref="A1:E1020"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -45078,7 +45078,7 @@
   <sheetPr codeName="Hoja5"/>
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
@@ -45578,26 +45578,13 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<Application xmlns="http://www.sap.com/cof/excel/application">
+  <Version>2</Version>
+  <Revision>2.3.1.59180</Revision>
+</Application>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="31c71105-5774-4818-b3e9-ee373a55139a" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="988afef9-5106-4784-a05b-d6b17e833319">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D7D51ED59FD6734BB27686473F8FE471" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="00dc82121fca9497ead1c88a6d6e1cd9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="988afef9-5106-4784-a05b-d6b17e833319" xmlns:ns3="31c71105-5774-4818-b3e9-ee373a55139a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6925f158d4a78352bd9b16e7cb8981ac" ns2:_="" ns3:_="">
     <xsd:import namespace="988afef9-5106-4784-a05b-d6b17e833319"/>
@@ -45826,39 +45813,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="31c71105-5774-4818-b3e9-ee373a55139a" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="988afef9-5106-4784-a05b-d6b17e833319">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<Application xmlns="http://www.sap.com/cof/excel/application">
-  <Version>2</Version>
-  <Revision>2.3.1.59180</Revision>
-</Application>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7384D329-D49C-4E31-809A-205D0FF28293}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0BE827E-7ABB-4702-AB9A-4F8E161605DE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.sap.com/cof/excel/application"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2D38E41-A563-47BB-9F03-424752BBF4BC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="988afef9-5106-4784-a05b-d6b17e833319"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="31c71105-5774-4818-b3e9-ee373a55139a"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{968DBFD8-121A-4A80-8F6C-87EF12B20096}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -45877,10 +45860,27 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2D38E41-A563-47BB-9F03-424752BBF4BC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="988afef9-5106-4784-a05b-d6b17e833319"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="31c71105-5774-4818-b3e9-ee373a55139a"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0BE827E-7ABB-4702-AB9A-4F8E161605DE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7384D329-D49C-4E31-809A-205D0FF28293}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.sap.com/cof/excel/application"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
refactor: Convertir codigos en funciones para correr en main.py
</commit_message>
<xml_diff>
--- a/data/segmentacion.xlsx
+++ b/data/segmentacion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sebatoec/projects/plantilla_seguimiento/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6895AEDE-472D-E641-94ED-39D8F004E723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{640B724F-F935-F44C-B4C4-A1C70D3E3C45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17340" activeTab="4" xr2:uid="{50E09FA1-93C2-8744-880E-4EAF34B822D2}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="add_spe_Polizas" sheetId="8" r:id="rId1"/>
     <sheet name="add_spe_Canales" sheetId="9" r:id="rId2"/>
     <sheet name="add_spe_Amparos" sheetId="1" r:id="rId3"/>
-    <sheet name="add_spe_Serfi" sheetId="11" r:id="rId4"/>
-    <sheet name="add_s_Atipicos" sheetId="13" r:id="rId5"/>
+    <sheet name="add_s_Atipicos" sheetId="13" r:id="rId4"/>
+    <sheet name="add_spe_Serfi" sheetId="11" r:id="rId5"/>
     <sheet name="Fechas" sheetId="12" r:id="rId6"/>
     <sheet name="Cuadre_Contable_Siniestros" sheetId="14" r:id="rId7"/>
     <sheet name="Cuadre_Contable_Primas" sheetId="15" r:id="rId8"/>
@@ -3673,7 +3673,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -3762,7 +3762,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -3785,7 +3785,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -27486,233 +27486,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBDCF800-6C43-45F5-A22F-852844811B3D}">
-  <sheetPr codeName="Hoja4"/>
-  <dimension ref="A1:C18"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B2" t="s">
-        <v>275</v>
-      </c>
-      <c r="C2" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B3" t="s">
-        <v>276</v>
-      </c>
-      <c r="C3" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B4" t="s">
-        <v>277</v>
-      </c>
-      <c r="C4" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B5" t="s">
-        <v>278</v>
-      </c>
-      <c r="C5" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B6" t="s">
-        <v>279</v>
-      </c>
-      <c r="C6" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>53</v>
-      </c>
-      <c r="B7" t="s">
-        <v>280</v>
-      </c>
-      <c r="C7" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8" t="s">
-        <v>281</v>
-      </c>
-      <c r="C8" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>53</v>
-      </c>
-      <c r="B9" t="s">
-        <v>282</v>
-      </c>
-      <c r="C9" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>53</v>
-      </c>
-      <c r="B10" t="s">
-        <v>283</v>
-      </c>
-      <c r="C10" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B11" t="s">
-        <v>284</v>
-      </c>
-      <c r="C11" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>53</v>
-      </c>
-      <c r="B12" t="s">
-        <v>285</v>
-      </c>
-      <c r="C12" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>53</v>
-      </c>
-      <c r="B13" t="s">
-        <v>286</v>
-      </c>
-      <c r="C13" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>53</v>
-      </c>
-      <c r="B14" t="s">
-        <v>287</v>
-      </c>
-      <c r="C14" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>53</v>
-      </c>
-      <c r="B15" t="s">
-        <v>288</v>
-      </c>
-      <c r="C15" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>53</v>
-      </c>
-      <c r="B16" t="s">
-        <v>289</v>
-      </c>
-      <c r="C16" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>53</v>
-      </c>
-      <c r="B17" t="s">
-        <v>290</v>
-      </c>
-      <c r="C17" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>53</v>
-      </c>
-      <c r="B18" t="s">
-        <v>291</v>
-      </c>
-      <c r="C18" t="s">
-        <v>296</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <customProperties>
-    <customPr name="_pios_id" r:id="rId1"/>
-  </customProperties>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC3B31F5-10E2-4C32-893C-13F98F395453}">
   <sheetPr codeName="Hoja6"/>
   <dimension ref="A1:E1020"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -45063,6 +44841,228 @@
       </c>
       <c r="E1020" s="10">
         <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <customProperties>
+    <customPr name="_pios_id" r:id="rId1"/>
+  </customProperties>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBDCF800-6C43-45F5-A22F-852844811B3D}">
+  <sheetPr codeName="Hoja4"/>
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" t="s">
+        <v>275</v>
+      </c>
+      <c r="C2" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" t="s">
+        <v>276</v>
+      </c>
+      <c r="C3" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" t="s">
+        <v>277</v>
+      </c>
+      <c r="C4" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" t="s">
+        <v>278</v>
+      </c>
+      <c r="C5" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" t="s">
+        <v>279</v>
+      </c>
+      <c r="C6" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" t="s">
+        <v>280</v>
+      </c>
+      <c r="C7" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" t="s">
+        <v>281</v>
+      </c>
+      <c r="C8" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" t="s">
+        <v>282</v>
+      </c>
+      <c r="C9" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" t="s">
+        <v>283</v>
+      </c>
+      <c r="C10" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" t="s">
+        <v>284</v>
+      </c>
+      <c r="C11" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" t="s">
+        <v>285</v>
+      </c>
+      <c r="C12" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" t="s">
+        <v>286</v>
+      </c>
+      <c r="C13" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" t="s">
+        <v>287</v>
+      </c>
+      <c r="C14" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" t="s">
+        <v>288</v>
+      </c>
+      <c r="C15" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" t="s">
+        <v>289</v>
+      </c>
+      <c r="C16" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" t="s">
+        <v>290</v>
+      </c>
+      <c r="C17" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" t="s">
+        <v>291</v>
+      </c>
+      <c r="C18" t="s">
+        <v>296</v>
       </c>
     </row>
   </sheetData>
@@ -45578,13 +45578,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<Application xmlns="http://www.sap.com/cof/excel/application">
-  <Version>2</Version>
-  <Revision>2.3.1.59180</Revision>
-</Application>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="31c71105-5774-4818-b3e9-ee373a55139a" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="988afef9-5106-4784-a05b-d6b17e833319">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D7D51ED59FD6734BB27686473F8FE471" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="00dc82121fca9497ead1c88a6d6e1cd9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="988afef9-5106-4784-a05b-d6b17e833319" xmlns:ns3="31c71105-5774-4818-b3e9-ee373a55139a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6925f158d4a78352bd9b16e7cb8981ac" ns2:_="" ns3:_="">
     <xsd:import namespace="988afef9-5106-4784-a05b-d6b17e833319"/>
@@ -45813,35 +45826,39 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="31c71105-5774-4818-b3e9-ee373a55139a" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="988afef9-5106-4784-a05b-d6b17e833319">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<Application xmlns="http://www.sap.com/cof/excel/application">
+  <Version>2</Version>
+  <Revision>2.3.1.59180</Revision>
+</Application>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0BE827E-7ABB-4702-AB9A-4F8E161605DE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7384D329-D49C-4E31-809A-205D0FF28293}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.sap.com/cof/excel/application"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2D38E41-A563-47BB-9F03-424752BBF4BC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="988afef9-5106-4784-a05b-d6b17e833319"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="31c71105-5774-4818-b3e9-ee373a55139a"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{968DBFD8-121A-4A80-8F6C-87EF12B20096}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -45860,27 +45877,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2D38E41-A563-47BB-9F03-424752BBF4BC}">
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0BE827E-7ABB-4702-AB9A-4F8E161605DE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="988afef9-5106-4784-a05b-d6b17e833319"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="31c71105-5774-4818-b3e9-ee373a55139a"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7384D329-D49C-4E31-809A-205D0FF28293}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.sap.com/cof/excel/application"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>